<commit_message>
Updated specifications with correct ID lengths
</commit_message>
<xml_diff>
--- a/source_data/STDSPECS_MinimumDataset.xlsx
+++ b/source_data/STDSPECS_MinimumDataset.xlsx
@@ -2044,7 +2044,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2080,7 +2080,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2660,10 +2659,10 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,7 +2672,7 @@
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="21" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" style="8" customWidth="1"/>
     <col min="8" max="8" width="11" style="8" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
@@ -2751,8 +2750,8 @@
       <c r="E2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="21">
-        <v>7</v>
+      <c r="F2" s="22">
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>35</v>
@@ -2818,7 +2817,7 @@
         <v>57</v>
       </c>
       <c r="F4" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>35</v>
@@ -3111,8 +3110,8 @@
       <c r="E13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="23">
-        <v>10</v>
+      <c r="F13" s="22">
+        <v>8</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>35</v>
@@ -3143,8 +3142,8 @@
       <c r="E14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="23">
-        <v>5</v>
+      <c r="F14" s="22">
+        <v>2</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>35</v>
@@ -3177,8 +3176,8 @@
       <c r="E15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="23">
-        <v>20</v>
+      <c r="F15" s="22">
+        <v>19</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>35</v>
@@ -3209,7 +3208,7 @@
       <c r="E16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="25">
         <v>8</v>
       </c>
       <c r="H16" s="8" t="s">
@@ -3244,7 +3243,7 @@
       <c r="E17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="22">
         <v>50</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -3278,7 +3277,7 @@
       <c r="E18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="22">
         <v>50</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -3312,7 +3311,7 @@
       <c r="E19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="23">
         <v>8</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -3346,7 +3345,7 @@
       <c r="E20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="23">
         <v>100</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -3380,7 +3379,7 @@
       <c r="E21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="22">
         <v>30</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -3412,7 +3411,7 @@
       <c r="E22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="23">
         <v>8</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -3444,7 +3443,7 @@
       <c r="E23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="23">
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -3476,7 +3475,7 @@
       <c r="E24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="26">
         <v>8</v>
       </c>
       <c r="H24" s="8" t="s">
@@ -3511,7 +3510,7 @@
       <c r="E25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="23">
         <v>20</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -3543,7 +3542,7 @@
       <c r="E26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="24"/>
+      <c r="F26" s="23"/>
       <c r="G26" s="7"/>
       <c r="H26" s="8" t="s">
         <v>70</v>
@@ -3577,7 +3576,7 @@
       <c r="E27" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="26">
         <v>8</v>
       </c>
       <c r="H27" s="8" t="s">
@@ -3612,8 +3611,8 @@
       <c r="E28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="27">
-        <v>20</v>
+      <c r="F28" s="26">
+        <v>19</v>
       </c>
       <c r="G28" s="7"/>
       <c r="I28" s="1" t="s">
@@ -3645,8 +3644,8 @@
       <c r="E29" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="25">
-        <v>10</v>
+      <c r="F29" s="22">
+        <v>8</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>35</v>
@@ -3677,8 +3676,8 @@
       <c r="E30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="25">
-        <v>5</v>
+      <c r="F30" s="1">
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>35</v>
@@ -3711,8 +3710,8 @@
       <c r="E31" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="25">
-        <v>20</v>
+      <c r="F31" s="24">
+        <v>19</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>35</v>
@@ -3743,7 +3742,7 @@
       <c r="E32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="27">
         <v>8</v>
       </c>
       <c r="H32" s="8" t="s">
@@ -3778,7 +3777,7 @@
       <c r="E33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="24">
         <v>8</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -3812,7 +3811,7 @@
       <c r="E34" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="27">
         <v>100</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -3846,7 +3845,7 @@
       <c r="E35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="24">
         <v>20</v>
       </c>
       <c r="I35" s="5" t="s">
@@ -3878,7 +3877,7 @@
       <c r="E36" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="24">
         <v>100</v>
       </c>
       <c r="I36" s="5" t="s">
@@ -3910,7 +3909,7 @@
       <c r="E37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="24">
         <v>20</v>
       </c>
       <c r="I37" s="5" t="s">
@@ -3942,7 +3941,7 @@
       <c r="E38" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="25">
+      <c r="F38" s="24">
         <v>100</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -3974,7 +3973,7 @@
       <c r="E39" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F39" s="28">
+      <c r="F39" s="27">
         <v>8</v>
       </c>
       <c r="H39" s="8" t="s">
@@ -4009,7 +4008,7 @@
       <c r="E40" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="25">
+      <c r="F40" s="24">
         <v>20</v>
       </c>
       <c r="I40" s="5" t="s">
@@ -11506,7 +11505,7 @@
       <c r="E232" s="17">
         <v>1</v>
       </c>
-      <c r="F232" s="29" t="s">
+      <c r="F232" s="28" t="s">
         <v>324</v>
       </c>
       <c r="G232" s="17"/>
@@ -11649,7 +11648,7 @@
       <c r="E238" s="17">
         <v>7</v>
       </c>
-      <c r="F238" s="30" t="s">
+      <c r="F238" s="29" t="s">
         <v>330</v>
       </c>
       <c r="L238" s="8"/>
@@ -11667,7 +11666,7 @@
       <c r="E239" s="17">
         <v>8</v>
       </c>
-      <c r="F239" s="30" t="s">
+      <c r="F239" s="29" t="s">
         <v>331</v>
       </c>
       <c r="L239" s="8"/>
@@ -11685,7 +11684,7 @@
       <c r="E240" s="17">
         <v>9</v>
       </c>
-      <c r="F240" s="30" t="s">
+      <c r="F240" s="29" t="s">
         <v>332</v>
       </c>
       <c r="L240" s="8"/>
@@ -11703,7 +11702,7 @@
       <c r="E241" s="17">
         <v>10</v>
       </c>
-      <c r="F241" s="30" t="s">
+      <c r="F241" s="29" t="s">
         <v>333</v>
       </c>
       <c r="L241" s="8"/>
@@ -11721,7 +11720,7 @@
       <c r="E242" s="17">
         <v>11</v>
       </c>
-      <c r="F242" s="30" t="s">
+      <c r="F242" s="29" t="s">
         <v>334</v>
       </c>
       <c r="L242" s="8"/>
@@ -11739,7 +11738,7 @@
       <c r="E243" s="17">
         <v>12</v>
       </c>
-      <c r="F243" s="31" t="s">
+      <c r="F243" s="30" t="s">
         <v>335</v>
       </c>
       <c r="L243" s="8"/>
@@ -11757,7 +11756,7 @@
       <c r="E244" s="17">
         <v>13</v>
       </c>
-      <c r="F244" s="32" t="s">
+      <c r="F244" s="31" t="s">
         <v>336</v>
       </c>
       <c r="L244" s="8"/>
@@ -11775,7 +11774,7 @@
       <c r="E245" s="17">
         <v>14</v>
       </c>
-      <c r="F245" s="31" t="s">
+      <c r="F245" s="30" t="s">
         <v>337</v>
       </c>
       <c r="L245" s="8"/>
@@ -17592,7 +17591,7 @@
         <v>486</v>
       </c>
       <c r="J490" s="17"/>
-      <c r="L490" s="33"/>
+      <c r="L490" s="32"/>
     </row>
     <row r="491" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">

</xml_diff>